<commit_message>
Development to Exploratory Analysis
Preparing the data to try to preliminarily answer questions
</commit_message>
<xml_diff>
--- a/Colorado_ACLU/2-jail-pop-trends-analysis/colorado-incarceration-hist.xlsx
+++ b/Colorado_ACLU/2-jail-pop-trends-analysis/colorado-incarceration-hist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SamPowers/Documents/GitHub/incarceration-trends/Colorado_ACLU/2-jail-pop-trends-analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13240" activeTab="2"/>
+    <workbookView xWindow="2980" yWindow="2540" windowWidth="24480" windowHeight="13240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +18,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,9 +29,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>* our data point is from Nov 27, all others are from December 31</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Jail Population</t>
   </si>
 </sst>
 </file>
@@ -362,15 +376,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -378,7 +400,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -386,7 +408,7 @@
         <v>1460.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -394,7 +416,7 @@
         <v>1487.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -402,7 +424,7 @@
         <v>1514.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -410,7 +432,7 @@
         <v>1541.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -418,7 +440,7 @@
         <v>1568.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -426,7 +448,7 @@
         <v>1595.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -434,7 +456,7 @@
         <v>1622.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -442,7 +464,7 @@
         <v>1602.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -450,7 +472,7 @@
         <v>1823.2</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -458,7 +480,7 @@
         <v>2044.9</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -466,7 +488,7 @@
         <v>2266.6</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1982</v>
       </c>
@@ -474,7 +496,7 @@
         <v>2488.3000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1983</v>
       </c>
@@ -482,7 +504,7 @@
         <v>2707</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1984</v>
       </c>
@@ -490,7 +512,7 @@
         <v>2880.9</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1985</v>
       </c>
@@ -498,7 +520,7 @@
         <v>3050.9</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1986</v>
       </c>
@@ -506,7 +528,7 @@
         <v>3715.4</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1987</v>
       </c>
@@ -514,7 +536,7 @@
         <v>4113.6000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1988</v>
       </c>
@@ -522,7 +544,7 @@
         <v>4352.8999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1989</v>
       </c>
@@ -530,7 +552,7 @@
         <v>5218.3999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -538,7 +560,7 @@
         <v>5618.4</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1991</v>
       </c>
@@ -546,7 +568,7 @@
         <v>5388.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1992</v>
       </c>
@@ -554,7 +576,7 @@
         <v>5417.3</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -562,7 +584,7 @@
         <v>6309.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1994</v>
       </c>
@@ -570,7 +592,7 @@
         <v>6554.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1995</v>
       </c>
@@ -578,7 +600,7 @@
         <v>7708.8</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1996</v>
       </c>
@@ -586,7 +608,7 @@
         <v>7481.4</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1997</v>
       </c>
@@ -594,7 +616,7 @@
         <v>8025.1</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1998</v>
       </c>
@@ -602,7 +624,7 @@
         <v>8166.7</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1999</v>
       </c>
@@ -610,7 +632,7 @@
         <v>8086.4</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -618,7 +640,7 @@
         <v>8238</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -626,7 +648,7 @@
         <v>8821.4</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2002</v>
       </c>
@@ -634,7 +656,7 @@
         <v>9756.9</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2003</v>
       </c>
@@ -642,7 +664,7 @@
         <v>10509.7</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2004</v>
       </c>
@@ -650,7 +672,7 @@
         <v>10864</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -658,7 +680,7 @@
         <v>12348.7</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2006</v>
       </c>
@@ -666,7 +688,7 @@
         <v>13185.6</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -674,7 +696,7 @@
         <v>12565.4</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2008</v>
       </c>
@@ -682,7 +704,7 @@
         <v>12076.4</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2009</v>
       </c>
@@ -690,7 +712,7 @@
         <v>11867.4</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2010</v>
       </c>
@@ -698,7 +720,7 @@
         <v>11623.6</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2011</v>
       </c>
@@ -706,7 +728,7 @@
         <v>11567.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2012</v>
       </c>
@@ -714,7 +736,7 @@
         <v>11023.9</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2013</v>
       </c>
@@ -722,7 +744,7 @@
         <v>11843</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -730,7 +752,7 @@
         <v>12115.5</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -738,12 +760,12 @@
         <v>11656</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2017</v>
       </c>
@@ -756,11 +778,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -770,14 +787,9 @@
   <sheetViews>
     <sheetView topLeftCell="A135" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -785,15 +797,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>